<commit_message>
Added reading exercise 2
</commit_message>
<xml_diff>
--- a/reading.xlsx
+++ b/reading.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="800" yWindow="460" windowWidth="24800" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="820" yWindow="460" windowWidth="24780" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="102">
   <si>
     <t>Exercise 1</t>
   </si>
@@ -86,18 +87,12 @@
     <t>C -&gt; AC</t>
   </si>
   <si>
-    <t>I don't know this question has multiple answers.</t>
-  </si>
-  <si>
     <t>Orbital parameters are conditions on Earth itself.</t>
   </si>
   <si>
     <t>B -&gt; E</t>
   </si>
   <si>
-    <t>~25</t>
-  </si>
-  <si>
     <t>%</t>
   </si>
   <si>
@@ -168,6 +163,177 @@
   </si>
   <si>
     <t>倾斜的</t>
+  </si>
+  <si>
+    <t>I didn't know this question has multiple answers.</t>
+  </si>
+  <si>
+    <t>Exercise 2</t>
+  </si>
+  <si>
+    <t>3'20''</t>
+  </si>
+  <si>
+    <t>~25'</t>
+  </si>
+  <si>
+    <t>2'10''</t>
+  </si>
+  <si>
+    <t>4'37''</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>3'36''</t>
+  </si>
+  <si>
+    <t>8'00''</t>
+  </si>
+  <si>
+    <t>E -&gt; A</t>
+  </si>
+  <si>
+    <t>E -&gt; C</t>
+  </si>
+  <si>
+    <t>10/12</t>
+  </si>
+  <si>
+    <t>21'72''</t>
+  </si>
+  <si>
+    <t>If the level had been much higher, then SO2 would not be necessarily generated.</t>
+  </si>
+  <si>
+    <t>clay</t>
+  </si>
+  <si>
+    <t>黏土</t>
+  </si>
+  <si>
+    <t>oxidize</t>
+  </si>
+  <si>
+    <t>氧化</t>
+  </si>
+  <si>
+    <t>discourse</t>
+  </si>
+  <si>
+    <t>论述，辩论</t>
+  </si>
+  <si>
+    <t>sulfur</t>
+  </si>
+  <si>
+    <t>硫</t>
+  </si>
+  <si>
+    <t>peasantry</t>
+  </si>
+  <si>
+    <t>农民</t>
+  </si>
+  <si>
+    <t>topography</t>
+  </si>
+  <si>
+    <t>地形</t>
+  </si>
+  <si>
+    <t>I misunderstood the meaning of "overlook." It means "ignore."</t>
+  </si>
+  <si>
+    <t>engender</t>
+  </si>
+  <si>
+    <t>导致</t>
+  </si>
+  <si>
+    <t>subsistence</t>
+  </si>
+  <si>
+    <t>维持生计</t>
+  </si>
+  <si>
+    <t>manifest</t>
+  </si>
+  <si>
+    <t>明显的</t>
+  </si>
+  <si>
+    <t>marmoset</t>
+  </si>
+  <si>
+    <t>狨</t>
+  </si>
+  <si>
+    <t>tamarin</t>
+  </si>
+  <si>
+    <t>小绢猴</t>
+  </si>
+  <si>
+    <t>stagger</t>
+  </si>
+  <si>
+    <t>蹒跚</t>
+  </si>
+  <si>
+    <t>paternity</t>
+  </si>
+  <si>
+    <t>父亲身份</t>
+  </si>
+  <si>
+    <t>facultive</t>
+  </si>
+  <si>
+    <t>自愿的</t>
+  </si>
+  <si>
+    <t>extant</t>
+  </si>
+  <si>
+    <t>尚存的</t>
+  </si>
+  <si>
+    <t>fate</t>
+  </si>
+  <si>
+    <t>命运</t>
+  </si>
+  <si>
+    <t>untenable</t>
+  </si>
+  <si>
+    <t>站不住脚的</t>
+  </si>
+  <si>
+    <t>incontestable</t>
+  </si>
+  <si>
+    <t>无可争辩的</t>
+  </si>
+  <si>
+    <t>immaterial</t>
+  </si>
+  <si>
+    <t>无关紧要的</t>
+  </si>
+  <si>
+    <t>conflate</t>
+  </si>
+  <si>
+    <t>合并，混淆</t>
+  </si>
+  <si>
+    <t>overlook</t>
+  </si>
+  <si>
+    <t>忽略</t>
   </si>
 </sst>
 </file>
@@ -491,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -536,7 +702,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -595,7 +761,7 @@
         <v>16</v>
       </c>
       <c r="J6" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -609,7 +775,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
         <v>17</v>
@@ -618,106 +784,384 @@
         <v>15</v>
       </c>
       <c r="J7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>37</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>39</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>41</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>43</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>46</v>
+      </c>
+      <c r="B22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" t="s">
+        <v>15</v>
+      </c>
+      <c r="J27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>94</v>
+      </c>
+      <c r="B47" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>